<commit_message>
Entiteettimalli tehty uudelleen, eka ei toiminut. Valocontrollerin luontia, ei valmis.
</commit_message>
<xml_diff>
--- a/SQL-taulut.xlsx
+++ b/SQL-taulut.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
-    <t>ValonMäärä</t>
-  </si>
-  <si>
     <t>SaunaID</t>
   </si>
   <si>
@@ -36,21 +33,6 @@
     <t>Valo100</t>
   </si>
   <si>
-    <t>ValoON</t>
-  </si>
-  <si>
-    <t>ValoOFF</t>
-  </si>
-  <si>
-    <t>ValoAika33</t>
-  </si>
-  <si>
-    <t>ValoAika66</t>
-  </si>
-  <si>
-    <t>ValoAika100</t>
-  </si>
-  <si>
     <t>SaunaNimi</t>
   </si>
   <si>
@@ -88,6 +70,24 @@
   </si>
   <si>
     <t>ValaisinNimi</t>
+  </si>
+  <si>
+    <t>Valo</t>
+  </si>
+  <si>
+    <t>ValoAikaLeima33</t>
+  </si>
+  <si>
+    <t>ValoAikaLeima66</t>
+  </si>
+  <si>
+    <t>ValoAikaLeima100</t>
+  </si>
+  <si>
+    <t>ValoAikaLeimaONOFF</t>
+  </si>
+  <si>
+    <t>ValoONOFF</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.8" x14ac:dyDescent="0.3"/>
@@ -466,65 +466,65 @@
     <col min="1" max="1" width="8.88671875" style="5"/>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" style="5"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="5"/>
     <col min="8" max="8" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2"/>
       <c r="H6" s="2"/>
@@ -543,28 +543,28 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="E10" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="D11" s="5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>7</v>
+      <c r="E13" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -581,30 +581,30 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E16" s="3" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E17" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E18" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E19" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>